<commit_message>
Updates from Catalina - Added some ship and vessel info
</commit_message>
<xml_diff>
--- a/Multibeam_metadata.xlsx
+++ b/Multibeam_metadata.xlsx
@@ -3932,6 +3932,14 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>Kongsberg Simrad EM3000</t>
+        </is>
+      </c>
+      <c r="P60">
+        <v>300</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -3990,6 +3998,14 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>Kongsberg Simrad EM3000</t>
+        </is>
+      </c>
+      <c r="P61">
+        <v>300</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -4038,6 +4054,19 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>R/V Suncoaster</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>Kongsberg Simrad EM3000</t>
+        </is>
+      </c>
+      <c r="P62">
+        <v>300</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -4091,6 +4120,19 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>R/V Suncoaster</t>
+        </is>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>Kongsberg Simrad EM3000</t>
+        </is>
+      </c>
+      <c r="P63">
+        <v>300</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -6669,6 +6711,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O104" t="inlineStr">
+        <is>
+          <t>Kongsberg Dual-head EM3000</t>
+        </is>
+      </c>
+      <c r="P104">
+        <v>300</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -6727,6 +6782,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O105" t="inlineStr">
+        <is>
+          <t>Kongsberg Dual-head EM3000</t>
+        </is>
+      </c>
+      <c r="P105">
+        <v>300</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -6785,6 +6853,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O106" t="inlineStr">
+        <is>
+          <t>Kongsberg Dual-head EM3000</t>
+        </is>
+      </c>
+      <c r="P106">
+        <v>300</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -6843,6 +6924,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>Kongsberg Dual-head EM3000</t>
+        </is>
+      </c>
+      <c r="P107">
+        <v>300</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -6901,6 +6995,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O108" t="inlineStr">
+        <is>
+          <t>Kongsberg Dual-head EM3000</t>
+        </is>
+      </c>
+      <c r="P108">
+        <v>300</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -6959,6 +7066,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>Kongsberg Dual-head EM3000</t>
+        </is>
+      </c>
+      <c r="P109">
+        <v>300</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -7118,6 +7238,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>R/V's Bellows &amp; Suncoaster</t>
+        </is>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>Kongsberg Simrad EM3000</t>
+        </is>
+      </c>
+      <c r="P112">
+        <v>300</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -7138,6 +7271,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>R/V's Bellows &amp; Suncoaster</t>
+        </is>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>Kongsberg Simrad EM3000</t>
+        </is>
+      </c>
+      <c r="P113">
+        <v>300</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114">
@@ -7191,6 +7337,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O114" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P114">
+        <v>95</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -7244,6 +7403,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P115">
+        <v>95</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -7302,6 +7474,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P116">
+        <v>95</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -7360,6 +7545,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P117">
+        <v>95</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -7418,6 +7616,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P118">
+        <v>95</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -7476,6 +7687,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P119">
+        <v>95</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -7534,6 +7758,19 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P120">
+        <v>95</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -7591,6 +7828,19 @@
         <is>
           <t>USGS</t>
         </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>R/V Moana Wave</t>
+        </is>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>Kongsberg EM1002</t>
+        </is>
+      </c>
+      <c r="P121">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2019_04A/B - Add backscatter surfaces - Split ULNALedges2A into 2A and 2B - Update code to redraw polygon if filename changes
</commit_message>
<xml_diff>
--- a/Multibeam_metadata.xlsx
+++ b/Multibeam_metadata.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P121"/>
+  <dimension ref="A1:Q123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,6 +438,11 @@
           <t>Frequency_kHz</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Old_Server_Location</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -514,6 +519,11 @@
       <c r="P2">
         <v>400</v>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL1/Bathymetry/EL1_Bathymetry_CUBE_2m.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -590,6 +600,11 @@
       <c r="P3">
         <v>400</v>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL1/Backscatter/EL1_1mTimeSeriesBS_TrimmedtoMosaic_AVG800.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -666,6 +681,11 @@
       <c r="P4">
         <v>400</v>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/MS_Gap/Bathymetry/Madison_Swanson_Gap_2m_Swath_Bathy.bag</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -742,6 +762,11 @@
       <c r="P5">
         <v>400</v>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/MS_Gap/Backscatter/WBII2016_04_MadisonSwansonGap_Snippetgeotiff.tif</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -818,6 +843,11 @@
       <c r="P6">
         <v>400</v>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG1/Bathymetry/CUBE/SWFMGMay2016_2.5mCube.bag</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -894,6 +924,11 @@
       <c r="P7">
         <v>400</v>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG1/Backscatter/SWFMGMay2016_1mBackScatter.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -970,6 +1005,11 @@
       <c r="P8">
         <v>400</v>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG2/Bathymetry/Swath_Angle/SWFMG2June2016_2m.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -1046,6 +1086,11 @@
       <c r="P9">
         <v>400</v>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG2/Backscatter/SWFMG2June2016_1mBackScatter_cropped.tif</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -1122,6 +1167,11 @@
       <c r="P10">
         <v>400</v>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG3/Bathymetry/CUBE/SWFMG3July2016Cube_2m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -1198,6 +1248,11 @@
       <c r="P11">
         <v>400</v>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG3/Backscatter/SWFMG3July2016_1mBS.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -1274,6 +1329,11 @@
       <c r="P12">
         <v>400</v>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG4/Bathymetry/CUBE/SWFMG4Cube2m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -1350,6 +1410,11 @@
       <c r="P13">
         <v>400</v>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG4/Backscatter/SWFMG4BeamAverage1m.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -1413,6 +1478,11 @@
           <t>CSCAMP</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/EFMG/EFMG1/Bathymetry/EastFMG1mswathangleApril2017.bag</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -1519,6 +1589,11 @@
       <c r="P16">
         <v>400</v>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL2/Bathymetry/EL2_AGU.bag</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -1633,6 +1708,11 @@
       <c r="P18">
         <v>400</v>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG5/Bathymetry/SWFMG5_4mCUBEBathy.bag</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -1742,6 +1822,11 @@
       <c r="P20">
         <v>400</v>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG6_WFMG1/Bathymetry/Cube/WFMG_4mCUBEBathy.bag</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -1856,6 +1941,11 @@
       <c r="P22">
         <v>400</v>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL3/Bathymetry/EL3_4mSwathBathy.bag</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -1970,6 +2060,11 @@
       <c r="P24">
         <v>400</v>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG7_WFMG2/Bathymetry/WFMG2_4mSwathBathy.bag</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -2084,6 +2179,11 @@
       <c r="P26">
         <v>400</v>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL4/Bathymetry/201804Elbow2mSA.bag</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -2160,6 +2260,11 @@
       <c r="P27">
         <v>400</v>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL4/Backscatter/EL4BS1m.tiff</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -2228,6 +2333,11 @@
           <t>R/V Hogarth</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>1_Cruises/2018_07B_HOG_SWFMG/QimeraProject/2018-07B-HOG/Export/SWFMG1807_2m_Raw.bag</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -2331,6 +2441,11 @@
           <t>R/V Hogarth</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>1_Cruises/2018_08_HOG_SWFMG/QimeraProjects/2018-08-HOG/Export/1808-SWFMG_2m_Raw.bag</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -2434,6 +2549,11 @@
           <t>R/V Hogarth</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>1_Cruises/2018_08_HOG_SWFMG/QimeraProjects/2018-08-HOG/Export/Mustache_Ext.bag</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -2545,6 +2665,11 @@
       <c r="P34">
         <v>400</v>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL5/Bathymetry/1809_EL5_2mBathy_PRELIMINARY.bag</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -2659,6 +2784,11 @@
       <c r="P36">
         <v>400</v>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG8_WFMG3/Bathymetry/1809_WFMG3C_2mBathy_PRELIMINARY.bag</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -2760,6 +2890,11 @@
           <t>CSCAMP</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/SWFMG/SWFMG8_WFMG3/Bathymetry/1809_WFMG3D_2mBathy_PRELIMINARY.bag</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -2866,6 +3001,11 @@
       <c r="P40">
         <v>400</v>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL6/Bathymetry/EL6A_PRELIMINARY.bag</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -2985,6 +3125,11 @@
       <c r="P42">
         <v>400</v>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Elbow/EL6/Bathymetry/EL6B_PRELIMINARY.bag</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -3104,6 +3249,11 @@
       <c r="P44">
         <v>400</v>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/RADIUS_1/Bathymetry/RadiusStep1A_3m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -3129,6 +3279,39 @@
           <t>Backscatter</t>
         </is>
       </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04A_HOG/Multibeam/FMGT_Projects/RADIUS_1A.fmproj/Output/Mosaic/RADIUS_1A_BS_TS_43-47_1m/RADIUS_1A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>RADIUS_1A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
       <c r="M45" t="inlineStr">
         <is>
           <t>CSCAMP</t>
@@ -3223,6 +3406,11 @@
       <c r="P46">
         <v>400</v>
       </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/ULNA_1/Bathymetry/UlnaLedges1A_3m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -3248,6 +3436,39 @@
           <t>Backscatter</t>
         </is>
       </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04A_HOG/Multibeam/FMGT_Projects/ULNA_1A.fmproj/Output/Mosaic/ULNA_1A_BS_TS_43-47_1m/ULNA_1A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>ULNA_1A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
       <c r="M47" t="inlineStr">
         <is>
           <t>CSCAMP</t>
@@ -3342,6 +3563,11 @@
       <c r="P48">
         <v>400</v>
       </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/RADIUS_2/Bathymetry/RadiusStep_2A_3m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -3367,6 +3593,39 @@
           <t>Backscatter</t>
         </is>
       </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/FMGT_Projects/RADIUS_2A.fmproj/Output/Mosaic/RADIUS_2A_BS_TS_43-47_1m/RADIUS_2A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>RADIUS_2A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
       <c r="M49" t="inlineStr">
         <is>
           <t>CSCAMP</t>
@@ -3461,6 +3720,11 @@
       <c r="P50">
         <v>400</v>
       </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/ULBOW_1/Bathymetry/ULbow_1A_3m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -3486,6 +3750,39 @@
           <t>Backscatter</t>
         </is>
       </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/FMGT_Projects/ULBOW_1A.fmproj/Output/Mosaic/ULBOW_1A_BS_TS_43-47_1m/ULBOW_1A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>ULBOW_1A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
       <c r="M51" t="inlineStr">
         <is>
           <t>CSCAMP</t>
@@ -3580,6 +3877,11 @@
       <c r="P52">
         <v>400</v>
       </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/ULBOW_1/Bathymetry/ULbow_1B_3m.bag</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -3605,6 +3907,39 @@
           <t>Backscatter</t>
         </is>
       </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/FMGT_Projects/ULBOW_1B.fmproj/Output/Mosaic/ULBOW_1B_BS_TS_43-47_1m/ULBOW_1B_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>ULBOW_1B_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
       <c r="M53" t="inlineStr">
         <is>
           <t>CSCAMP</t>
@@ -3673,12 +4008,12 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/ULNA_2/Bathymetry/UlnaLedges_2A_3m.bag</t>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/Qimera_Project/2019-04B-WB2-CBASS/Export/ULNA_2A_3m.bag</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>UlnaLedges_2A_3m.bag</t>
+          <t>ULNA_2A_3m.bag</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
@@ -3698,6 +4033,11 @@
       </c>
       <c r="P54">
         <v>400</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/C_Multibeam_C-SCAMP/Radius_Ulna_Ulbow/ULNA_2/Bathymetry/UlnaLedges_2A_3m.bag</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -3724,6 +4064,39 @@
           <t>Backscatter</t>
         </is>
       </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/FMGT_Projects/ULNA_2A.fmproj/Output/Mosaic/ULNA_2A_BS_TS_43-47_1m/ULNA_2A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>ULNA_2A_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
       <c r="M55" t="inlineStr">
         <is>
           <t>CSCAMP</t>
@@ -3790,6 +4163,11 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/The_Edges_Seasonal_MPA/Bathymetry/TheEdges_2005_08_corridor_001.asc</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -3858,6 +4236,11 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Florida_Middle_Grounds_HAPC/Bathymetry/2006_fmg.asc</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -3911,6 +4294,11 @@
           <t>David Naar</t>
         </is>
       </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Florida_Middle_Grounds_HAPC/Backscatter/2006_07_fmg_5m_NAfixed.tif</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -3972,6 +4360,11 @@
       <c r="P60">
         <v>300</v>
       </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Madison_Swanson_MPA/NEcorner/Bathymetry/2002_madison_0001.asc</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -4038,6 +4431,11 @@
       <c r="P61">
         <v>300</v>
       </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Madison_Swanson_MPA/NEcorner/Backscatter/2002_07_Madison_5m_NAFixed.tif</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -4099,6 +4497,11 @@
       <c r="P62">
         <v>300</v>
       </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Twin_Ridges/Bathymetry/2002_twin_ridges_0001.asc</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -4165,6 +4568,11 @@
       <c r="P63">
         <v>300</v>
       </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Twin_Ridges/Backscatter/2002_07_twin_ridges_5m.tif</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -4228,6 +4636,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/761401_Florida_Trackline.asc</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -4291,6 +4704,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block181_4mSa.asc</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -4354,6 +4772,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block197_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -4417,6 +4840,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block240_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -4480,6 +4908,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block031E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -4543,6 +4976,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block032E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -4606,6 +5044,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block105E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -4669,6 +5112,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block125_145E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -4732,6 +5180,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block125E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -4795,6 +5248,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block125E_N.asc</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -4858,6 +5316,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block125E_S.asc</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -4921,6 +5384,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block145E.asc</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -4984,6 +5452,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block197E.asc</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -5047,6 +5520,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block226E_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -5110,6 +5588,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block238E_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -5173,6 +5656,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block240_D266_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -5236,6 +5724,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block240-227_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -5299,6 +5792,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block253E_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -5362,6 +5860,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block254a_Day264_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -5425,6 +5928,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block254b_Day264_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -5488,6 +5996,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block254c_Day264_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -5551,6 +6064,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block254d_Day264_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -5614,6 +6132,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block254E_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -5677,6 +6200,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block268_Day265_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -5740,6 +6268,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block296_Day264_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -5803,6 +6336,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block345E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -5866,6 +6404,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block371E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -5929,6 +6472,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block372E.asc</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -5992,6 +6540,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block372E_2.asc</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -6055,6 +6608,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block373E.asc</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -6118,6 +6676,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block403_Day262_CamSites_2m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -6181,6 +6744,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block403_Day263_CamSites_2m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -6244,6 +6812,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block404_Day263_CamSites_2m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -6307,6 +6880,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block405_Day262_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -6370,6 +6948,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block405_Day263_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -6433,6 +7016,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block423E_4m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -6496,6 +7084,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block495E_8m.asc</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -6559,6 +7152,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block525E.asc</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -6622,6 +7220,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block553E.asc</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -6685,6 +7288,11 @@
           <t>Simrad ME70</t>
         </is>
       </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/NOAA_NMFS_Surfaces_ME70/Block84E_5m_Cube.asc</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -6756,6 +7364,11 @@
       <c r="P104">
         <v>300</v>
       </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/DeSoto_Canyon/Bathymetry/Central_Bathymetry/cenbathg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -6827,6 +7440,11 @@
       <c r="P105">
         <v>300</v>
       </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/DeSoto_Canyon/Backscatter/Central_Backscatter/cenmosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -6898,6 +7516,11 @@
       <c r="P106">
         <v>300</v>
       </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/DeSoto_Canyon/Bathymetry/Northern_Bathymetry/nthbathg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -6969,6 +7592,11 @@
       <c r="P107">
         <v>300</v>
       </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/DeSoto_Canyon/Backscatter/Northern_Backscatter/nthmosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -7040,6 +7668,11 @@
       <c r="P108">
         <v>300</v>
       </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/DeSoto_Canyon/Bathymetry/Southern_Bathymetry/sthbathg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -7111,6 +7744,11 @@
       <c r="P109">
         <v>300</v>
       </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/DeSoto_Canyon/Backscatter/Southern_Backscatter/sthmosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -7164,6 +7802,11 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Pinnacles/Bathymetry/bathyg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111">
@@ -7217,6 +7860,11 @@
           <t>USGS</t>
         </is>
       </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Pinnacles/Backscatter/mosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112">
@@ -7283,6 +7931,11 @@
       <c r="P112">
         <v>300</v>
       </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Pulley_Ridge/Bathymetry/allpr_filcrop.asc</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -7382,6 +8035,11 @@
       <c r="P114">
         <v>95</v>
       </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Steamboat_Lumps_MPA/Bathymetry/sbbathyg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -7448,6 +8106,11 @@
       <c r="P115">
         <v>95</v>
       </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/Steamboat_Lumps_MPA/Backscatter/sbmosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -7519,6 +8182,11 @@
       <c r="P116">
         <v>95</v>
       </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/West_Florida_Shelf/Central/Bathymetry/cbathyg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -7590,6 +8258,11 @@
       <c r="P117">
         <v>95</v>
       </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/West_Florida_Shelf/Central/Backscatter/cmosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -7661,6 +8334,11 @@
       <c r="P118">
         <v>95</v>
       </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/West_Florida_Shelf/Northern/Bathymetry/nbathyg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -7732,6 +8410,11 @@
       <c r="P119">
         <v>95</v>
       </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/West_Florida_Shelf/Northern/Backscatter/nmosg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -7803,6 +8486,11 @@
       <c r="P120">
         <v>95</v>
       </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/West_Florida_Shelf/Southern/Bathymetry/sbathyg/w001001.adf</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -7873,6 +8561,163 @@
       </c>
       <c r="P121">
         <v>95</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>2_Projects/GIS/G_Multibeam_Other_Sources/West_Florida_Shelf/Southern/Backscatter/smosg/w001001.adf</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>ULNA</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2019_04B_WB2_CBASS</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Bathymetry</t>
+        </is>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>FPC_Universal_Transverse_Mercator_North_Hemisphere</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>GRS80</t>
+        </is>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/Qimera_Project/2019-04B-WB2-CBASS/Export/ULNA_2B_3m.bag</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>ULNA_2B_3m.bag</t>
+        </is>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>CSCAMP</t>
+        </is>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>R/V Weatherbird II</t>
+        </is>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>Teledyne Reson SeaBat T50-R Dual Head</t>
+        </is>
+      </c>
+      <c r="P122">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>ULNA</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2B</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2019_04B_WB2_CBASS</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Backscatter</t>
+        </is>
+      </c>
+      <c r="F123">
+        <v>1</v>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>WGS 84 / UTM zone 16N</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>utm 16</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>WGS84</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>1_Cruises/2019_04B_WB2_CBASS/Multibeam/FMGT_Projects/ULNA_2B.fmproj/Output/Mosaic/ULNA_2B_BS_TS_43-47_1m/ULNA_2B_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>ULNA_2B_BS_TS_43-47_1m.tif</t>
+        </is>
+      </c>
+      <c r="M123" t="inlineStr">
+        <is>
+          <t>CSCAMP</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>R/V Weatherbird II</t>
+        </is>
+      </c>
+      <c r="O123" t="inlineStr">
+        <is>
+          <t>Teledyne Reson SeaBat T50-R Dual Head</t>
+        </is>
+      </c>
+      <c r="P123">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Updates - Add more info to Readme to clarify where data is located - Change "D:" external drive paths to NFWF server path - Change C-SCAMP url to DOI of final report
</commit_message>
<xml_diff>
--- a/Multibeam_metadata.xlsx
+++ b/Multibeam_metadata.xlsx
@@ -547,7 +547,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -982,7 +982,7 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="T15" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="T19" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2209,7 +2209,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2296,7 +2296,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -2355,7 +2355,7 @@
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2534,7 +2534,7 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="T28" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>D:/Ilich/1_Cruises/2018_07B_HOG_SWFMG/FMGT_Projects/SWFMG_9.fmproj/Output/Mosaic/SWFMG_9_BS_TS_43-47_1m/SWFMG_9_BS_TS_43-47_1m.tif</t>
+          <t>1_Cruises/2018_07B_HOG_SWFMG/FMGT_Projects/SWFMG_9.fmproj/Output/Mosaic/SWFMG_9_BS_TS_43-47_1m/SWFMG_9_BS_TS_43-47_1m.tif</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2810,7 +2810,7 @@
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2874,7 +2874,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>D:/Ilich/1_Cruises/2018_08_HOG_SWFMG/FMGT_Projects/SWFMG_10A.fmproj/Output/Mosaic/SWFMG_10A_BS_TS_43-47_1m/SWFMG_10A_BS_TS_43-47_1m.tif</t>
+          <t>1_Cruises/2018_08_HOG_SWFMG/FMGT_Projects/SWFMG_10A.fmproj/Output/Mosaic/SWFMG_10A_BS_TS_43-47_1m/SWFMG_10A_BS_TS_43-47_1m.tif</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="T31" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -2994,7 +2994,7 @@
       </c>
       <c r="T32" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3058,7 +3058,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>D:/Ilich/1_Cruises/2018_08_HOG_SWFMG/FMGT_Projects/SWFMG_10B.fmproj/Output/Mosaic/SWFMG_10B_BS_TS_43-47_1m/SWFMG_10B_BS_TS_43-47_1m.tif</t>
+          <t>1_Cruises/2018_08_HOG_SWFMG/FMGT_Projects/SWFMG_10B.fmproj/Output/Mosaic/SWFMG_10B_BS_TS_43-47_1m/SWFMG_10B_BS_TS_43-47_1m.tif</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="T34" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3260,7 +3260,7 @@
       </c>
       <c r="T35" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="T36" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="T37" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3628,7 +3628,7 @@
       </c>
       <c r="T39" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3715,7 +3715,7 @@
       </c>
       <c r="T40" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="T41" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3889,7 +3889,7 @@
       </c>
       <c r="T42" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="T43" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="T45" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="T46" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4324,7 +4324,7 @@
       </c>
       <c r="T47" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4411,7 +4411,7 @@
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4585,7 +4585,7 @@
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="T51" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="T52" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="T53" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -4933,7 +4933,7 @@
       </c>
       <c r="T54" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -9429,7 +9429,7 @@
       </c>
       <c r="T122" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -9516,7 +9516,7 @@
       </c>
       <c r="T123" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -9608,7 +9608,7 @@
       </c>
       <c r="T124" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>
@@ -9700,7 +9700,7 @@
       </c>
       <c r="T125" t="inlineStr">
         <is>
-          <t>https://www.marine.usf.edu/scamp/</t>
+          <t>https://zenodo.org/doi/10.5281/zenodo.8381009</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix typos in sonar name - Fix typos in sonar names - Comit server - Remove perl=TRUE in regex b/c no longer works
</commit_message>
<xml_diff>
--- a/Multibeam_metadata.xlsx
+++ b/Multibeam_metadata.xlsx
@@ -1837,7 +1837,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>Teledyne Reson SeaBat 7126</t>
+          <t>Teledyne Reson SeaBat 7125</t>
         </is>
       </c>
       <c r="T16">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>Teledyne Reson SeaBat 7127</t>
+          <t>Teledyne Reson SeaBat 7125</t>
         </is>
       </c>
       <c r="T17">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>Teledyne Reson SeaBat 7126</t>
+          <t>Teledyne Reson SeaBat 7125</t>
         </is>
       </c>
       <c r="T22">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>Teledyne Reson SeaBat 7127</t>
+          <t>Teledyne Reson SeaBat 7125</t>
         </is>
       </c>
       <c r="T23">
@@ -10458,7 +10458,7 @@
       </c>
       <c r="S130" t="inlineStr">
         <is>
-          <t>Kongsberg Simrad EM 3000</t>
+          <t>Kongsberg Simrad EM3000</t>
         </is>
       </c>
       <c r="T130">
@@ -10509,7 +10509,7 @@
       </c>
       <c r="S131" t="inlineStr">
         <is>
-          <t>Kongsberg Simrad EM 3001</t>
+          <t>Kongsberg Simrad EM3000</t>
         </is>
       </c>
       <c r="T131">

</xml_diff>